<commit_message>
Committed merged AR Reporting Cases code - 29th Oct
</commit_message>
<xml_diff>
--- a/Test_Scenario/RIS_TestCase.xlsx
+++ b/Test_Scenario/RIS_TestCase.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="94">
   <si>
     <t>Steps</t>
   </si>
@@ -55,9 +55,6 @@
     <t>No run</t>
   </si>
   <si>
-    <t>Fail</t>
-  </si>
-  <si>
     <t xml:space="preserve">iproc Requistion creation, receving  </t>
   </si>
   <si>
@@ -104,6 +101,9 @@
   </si>
   <si>
     <t>Requisition with leasehold improvement: REAL ESTATE.DESIGN AND CONSTRUCTION.55121700 OR FM.Building Maintenance.26000000</t>
+  </si>
+  <si>
+    <t>Operational Reporting -MMC GLB AR Outstanding Invoices Listing</t>
   </si>
   <si>
     <t>TestCase_Id</t>
@@ -233,6 +233,9 @@
     <t>GSI.A2R.IP.03.003</t>
   </si>
   <si>
+    <t>fn_SubmitRequest</t>
+  </si>
+  <si>
     <t>fn_logout</t>
   </si>
   <si>
@@ -273,6 +276,9 @@
   </si>
   <si>
     <t>Pass</t>
+  </si>
+  <si>
+    <t>GSI.O2C.AR.SA.017</t>
   </si>
   <si>
     <t>Step 13</t>
@@ -332,7 +338,31 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -340,6 +370,51 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -355,52 +430,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -408,30 +437,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri Light"/>
-      <family val="2"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -505,7 +511,9 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -529,9 +537,7 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -560,18 +566,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
@@ -580,49 +586,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -892,10 +898,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G63"/>
+  <dimension ref="A1:G66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18:B24"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -903,7 +909,8 @@
     <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.6640625" style="18" customWidth="1"/>
     <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="38.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row>
@@ -917,10 +924,10 @@
         <v>0</v>
       </c>
       <c s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c s="4" t="s">
         <v>36</v>
@@ -930,57 +937,57 @@
       </c>
     </row>
     <row>
-      <c s="10" t="s">
+      <c s="8" t="s">
+        <v>80</v>
+      </c>
+      <c s="3" t="s">
+        <v>58</v>
+      </c>
+      <c s="1" t="s">
+        <v>67</v>
+      </c>
+      <c s="1" t="s">
+        <v>30</v>
+      </c>
+      <c s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G2" s="1"/>
+    </row>
+    <row>
+      <c s="8"/>
+      <c s="3"/>
+      <c s="1" t="s">
+        <v>88</v>
+      </c>
+      <c s="1" t="s">
+        <v>38</v>
+      </c>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+    </row>
+    <row>
+      <c s="8"/>
+      <c s="3"/>
+      <c s="1" t="s">
+        <v>20</v>
+      </c>
+      <c s="1" t="s">
+        <v>14</v>
+      </c>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+    </row>
+    <row>
+      <c s="8"/>
+      <c s="3"/>
+      <c s="1" t="s">
+        <v>43</v>
+      </c>
+      <c s="1" t="s">
         <v>79</v>
-      </c>
-      <c s="3" t="s">
-        <v>58</v>
-      </c>
-      <c s="1" t="s">
-        <v>67</v>
-      </c>
-      <c s="1" t="s">
-        <v>30</v>
-      </c>
-      <c s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="G2" s="1"/>
-    </row>
-    <row>
-      <c s="10"/>
-      <c s="3"/>
-      <c s="1" t="s">
-        <v>86</v>
-      </c>
-      <c s="1" t="s">
-        <v>38</v>
-      </c>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-    </row>
-    <row>
-      <c s="10"/>
-      <c s="3"/>
-      <c s="1" t="s">
-        <v>21</v>
-      </c>
-      <c s="1" t="s">
-        <v>15</v>
-      </c>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-    </row>
-    <row>
-      <c s="10"/>
-      <c s="3"/>
-      <c s="1" t="s">
-        <v>43</v>
-      </c>
-      <c s="1" t="s">
-        <v>78</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>68</v>
@@ -988,20 +995,20 @@
       <c s="1"/>
     </row>
     <row>
-      <c s="10"/>
+      <c s="8"/>
       <c s="3"/>
       <c s="1" t="s">
         <v>69</v>
       </c>
       <c t="s">
-        <v>24</v>
-      </c>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-    </row>
-    <row>
-      <c s="10" t="s">
+        <v>23</v>
+      </c>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+    </row>
+    <row>
+      <c s="8" t="s">
         <v>31</v>
       </c>
       <c s="9" t="s">
@@ -1020,10 +1027,10 @@
       <c s="2"/>
     </row>
     <row>
-      <c s="10"/>
+      <c s="8"/>
       <c s="9"/>
       <c s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c t="s">
         <v>4</v>
@@ -1035,24 +1042,24 @@
       <c s="2"/>
     </row>
     <row>
-      <c s="10"/>
+      <c s="8"/>
       <c s="9"/>
       <c s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c t="s">
-        <v>24</v>
-      </c>
-      <c s="2"/>
-      <c s="2"/>
-      <c s="2"/>
-    </row>
-    <row>
-      <c s="10" t="s">
+        <v>23</v>
+      </c>
+      <c s="2"/>
+      <c s="2"/>
+      <c s="2"/>
+    </row>
+    <row>
+      <c s="8" t="s">
         <v>53</v>
       </c>
       <c s="9" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c s="2" t="s">
         <v>67</v>
@@ -1067,10 +1074,10 @@
       <c s="2"/>
     </row>
     <row>
-      <c s="10"/>
+      <c s="8"/>
       <c s="9"/>
       <c s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c t="s">
         <v>4</v>
@@ -1082,24 +1089,24 @@
       <c s="2"/>
     </row>
     <row>
-      <c s="10"/>
+      <c s="8"/>
       <c s="9"/>
       <c s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c t="s">
-        <v>24</v>
-      </c>
-      <c s="2"/>
-      <c s="2"/>
-      <c s="2"/>
-    </row>
-    <row>
-      <c s="15" t="s">
-        <v>80</v>
-      </c>
-      <c s="22" t="s">
-        <v>16</v>
+        <v>23</v>
+      </c>
+      <c s="2"/>
+      <c s="2"/>
+      <c s="2"/>
+    </row>
+    <row>
+      <c s="13" t="s">
+        <v>81</v>
+      </c>
+      <c s="20" t="s">
+        <v>15</v>
       </c>
       <c s="2" t="s">
         <v>67</v>
@@ -1108,16 +1115,16 @@
         <v>30</v>
       </c>
       <c s="2" t="s">
-        <v>80</v>
-      </c>
-      <c s="2"/>
-      <c s="2"/>
-    </row>
-    <row>
-      <c s="13"/>
-      <c s="17"/>
-      <c s="2" t="s">
-        <v>86</v>
+        <v>81</v>
+      </c>
+      <c s="2"/>
+      <c s="2"/>
+    </row>
+    <row>
+      <c s="22"/>
+      <c s="21"/>
+      <c s="2" t="s">
+        <v>88</v>
       </c>
       <c t="s">
         <v>4</v>
@@ -1129,21 +1136,21 @@
       <c s="2"/>
     </row>
     <row>
-      <c s="13"/>
-      <c s="17"/>
-      <c s="2" t="s">
-        <v>21</v>
-      </c>
-      <c s="1" t="s">
-        <v>24</v>
-      </c>
-      <c s="2"/>
-      <c s="2"/>
-      <c s="2"/>
-    </row>
-    <row>
-      <c s="13"/>
-      <c s="17"/>
+      <c s="22"/>
+      <c s="21"/>
+      <c s="2" t="s">
+        <v>20</v>
+      </c>
+      <c s="1" t="s">
+        <v>23</v>
+      </c>
+      <c s="2"/>
+      <c s="2"/>
+      <c s="2"/>
+    </row>
+    <row>
+      <c s="22"/>
+      <c s="21"/>
       <c s="2" t="s">
         <v>43</v>
       </c>
@@ -1157,8 +1164,8 @@
       <c s="2"/>
     </row>
     <row>
-      <c s="13"/>
-      <c s="17"/>
+      <c s="22"/>
+      <c s="21"/>
       <c s="2" t="s">
         <v>69</v>
       </c>
@@ -1166,15 +1173,15 @@
         <v>59</v>
       </c>
       <c s="1"/>
-      <c s="11"/>
-      <c s="2"/>
-    </row>
-    <row>
-      <c s="10" t="s">
+      <c s="10"/>
+      <c s="2"/>
+    </row>
+    <row>
+      <c s="8" t="s">
         <v>8</v>
       </c>
       <c s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c s="2" t="s">
         <v>67</v>
@@ -1189,10 +1196,10 @@
       <c s="2"/>
     </row>
     <row>
-      <c s="10"/>
+      <c s="8"/>
       <c s="9"/>
       <c s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c t="s">
         <v>4</v>
@@ -1204,20 +1211,20 @@
       <c s="2"/>
     </row>
     <row>
-      <c s="10"/>
+      <c s="8"/>
       <c s="9"/>
       <c s="2" t="s">
-        <v>21</v>
-      </c>
-      <c s="1" t="s">
-        <v>24</v>
-      </c>
-      <c s="2"/>
-      <c s="2"/>
-      <c s="2"/>
-    </row>
-    <row>
-      <c s="10"/>
+        <v>20</v>
+      </c>
+      <c s="1" t="s">
+        <v>23</v>
+      </c>
+      <c s="2"/>
+      <c s="2"/>
+      <c s="2"/>
+    </row>
+    <row>
+      <c s="8"/>
       <c s="9"/>
       <c s="2" t="s">
         <v>43</v>
@@ -1232,41 +1239,41 @@
       <c s="2"/>
     </row>
     <row>
+      <c s="8"/>
+      <c s="9"/>
+      <c s="2" t="s">
+        <v>69</v>
+      </c>
+      <c s="1" t="s">
+        <v>59</v>
+      </c>
+      <c s="1"/>
       <c s="10"/>
+      <c s="2"/>
+    </row>
+    <row>
+      <c s="8"/>
       <c s="9"/>
       <c s="2" t="s">
-        <v>69</v>
-      </c>
-      <c s="1" t="s">
-        <v>59</v>
-      </c>
-      <c s="1"/>
-      <c s="11"/>
-      <c s="2"/>
-    </row>
-    <row>
-      <c s="10"/>
+        <v>91</v>
+      </c>
+      <c s="1" t="s">
+        <v>62</v>
+      </c>
+      <c s="2"/>
+      <c s="2" t="s">
+        <v>26</v>
+      </c>
+      <c s="2"/>
+    </row>
+    <row>
+      <c s="8"/>
       <c s="9"/>
       <c s="2" t="s">
-        <v>89</v>
-      </c>
-      <c s="1" t="s">
-        <v>62</v>
-      </c>
-      <c s="2"/>
-      <c s="2" t="s">
-        <v>27</v>
-      </c>
-      <c s="2"/>
-    </row>
-    <row>
-      <c s="10"/>
-      <c s="9"/>
-      <c s="2" t="s">
-        <v>26</v>
-      </c>
-      <c s="1" t="s">
-        <v>74</v>
+        <v>25</v>
+      </c>
+      <c s="1" t="s">
+        <v>75</v>
       </c>
       <c s="2"/>
       <c s="2"/>
@@ -1295,7 +1302,7 @@
       <c s="7"/>
       <c s="7"/>
       <c s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c s="1" t="s">
         <v>4</v>
@@ -1310,10 +1317,10 @@
       <c s="7"/>
       <c s="7"/>
       <c s="2" t="s">
-        <v>21</v>
-      </c>
-      <c s="1" t="s">
-        <v>24</v>
+        <v>20</v>
+      </c>
+      <c s="1" t="s">
+        <v>23</v>
       </c>
       <c s="2"/>
       <c s="2"/>
@@ -1351,22 +1358,22 @@
       <c s="7"/>
       <c s="7"/>
       <c s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c s="1" t="s">
         <v>62</v>
       </c>
       <c s="2"/>
       <c s="2" t="s">
-        <v>27</v>
-      </c>
-      <c s="1"/>
-    </row>
-    <row>
-      <c s="7"/>
-      <c s="7"/>
-      <c s="2" t="s">
         <v>26</v>
+      </c>
+      <c s="1"/>
+    </row>
+    <row>
+      <c s="7"/>
+      <c s="7"/>
+      <c s="2" t="s">
+        <v>25</v>
       </c>
       <c s="1" t="s">
         <v>50</v>
@@ -1398,7 +1405,7 @@
       <c s="7"/>
       <c s="7"/>
       <c s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c s="1" t="s">
         <v>4</v>
@@ -1413,10 +1420,10 @@
       <c s="7"/>
       <c s="7"/>
       <c s="2" t="s">
-        <v>21</v>
-      </c>
-      <c s="1" t="s">
-        <v>24</v>
+        <v>20</v>
+      </c>
+      <c s="1" t="s">
+        <v>23</v>
       </c>
       <c s="2"/>
       <c s="2"/>
@@ -1454,25 +1461,25 @@
       <c s="7"/>
       <c s="7"/>
       <c s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c s="1" t="s">
         <v>62</v>
       </c>
       <c s="2"/>
       <c s="2" t="s">
-        <v>27</v>
-      </c>
-      <c s="1"/>
-    </row>
-    <row>
-      <c s="7"/>
-      <c s="7"/>
-      <c s="2" t="s">
         <v>26</v>
       </c>
-      <c s="1" t="s">
-        <v>18</v>
+      <c s="1"/>
+    </row>
+    <row>
+      <c s="7"/>
+      <c s="7"/>
+      <c s="2" t="s">
+        <v>25</v>
+      </c>
+      <c s="1" t="s">
+        <v>17</v>
       </c>
       <c s="1"/>
       <c s="1"/>
@@ -1501,7 +1508,7 @@
       <c s="7"/>
       <c s="7"/>
       <c s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c s="1" t="s">
         <v>4</v>
@@ -1516,7 +1523,7 @@
       <c s="7"/>
       <c s="7"/>
       <c s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c s="1" t="s">
         <v>47</v>
@@ -1548,7 +1555,7 @@
       <c s="7"/>
       <c s="7"/>
       <c s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c s="1" t="s">
         <v>4</v>
@@ -1563,7 +1570,7 @@
       <c s="7"/>
       <c s="7"/>
       <c s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c s="1" t="s">
         <v>47</v>
@@ -1576,7 +1583,7 @@
       <c s="3" t="s">
         <v>10</v>
       </c>
-      <c s="19" t="s">
+      <c s="15" t="s">
         <v>64</v>
       </c>
       <c s="3" t="s">
@@ -1593,9 +1600,9 @@
     </row>
     <row>
       <c s="3"/>
-      <c s="19"/>
-      <c s="3" t="s">
-        <v>86</v>
+      <c s="15"/>
+      <c s="3" t="s">
+        <v>88</v>
       </c>
       <c s="1" t="s">
         <v>4</v>
@@ -1608,13 +1615,13 @@
     </row>
     <row>
       <c s="3"/>
-      <c s="19"/>
-      <c s="3" t="s">
-        <v>21</v>
-      </c>
-      <c s="1" t="s">
+      <c s="15"/>
+      <c s="3" t="s">
         <v>20</v>
       </c>
+      <c s="1" t="s">
+        <v>19</v>
+      </c>
       <c s="1"/>
       <c s="3" t="s">
         <v>65</v>
@@ -1623,7 +1630,7 @@
     </row>
     <row>
       <c s="3"/>
-      <c s="19"/>
+      <c s="15"/>
       <c s="3" t="s">
         <v>43</v>
       </c>
@@ -1638,38 +1645,38 @@
     </row>
     <row>
       <c s="3"/>
-      <c s="19"/>
+      <c s="15"/>
       <c s="3" t="s">
         <v>69</v>
       </c>
       <c s="1" t="s">
-        <v>24</v>
-      </c>
-      <c s="3"/>
-      <c s="1"/>
-      <c s="3"/>
-    </row>
-    <row>
-      <c s="3"/>
-      <c s="19"/>
-      <c s="3" t="s">
-        <v>89</v>
+        <v>23</v>
+      </c>
+      <c s="3"/>
+      <c s="1"/>
+      <c s="3"/>
+    </row>
+    <row>
+      <c s="3"/>
+      <c s="15"/>
+      <c s="3" t="s">
+        <v>91</v>
       </c>
       <c s="1" t="s">
         <v>62</v>
       </c>
       <c s="3"/>
       <c s="3" t="s">
-        <v>27</v>
-      </c>
-      <c s="3"/>
-    </row>
-    <row>
-      <c s="3"/>
-      <c s="19"/>
-      <c s="3" t="s">
         <v>26</v>
       </c>
+      <c s="3"/>
+    </row>
+    <row>
+      <c s="3"/>
+      <c s="15"/>
+      <c s="3" t="s">
+        <v>25</v>
+      </c>
       <c s="1" t="s">
         <v>59</v>
       </c>
@@ -1679,7 +1686,7 @@
     </row>
     <row>
       <c s="3"/>
-      <c s="19"/>
+      <c s="15"/>
       <c s="3" t="s">
         <v>49</v>
       </c>
@@ -1694,20 +1701,20 @@
     </row>
     <row>
       <c s="3"/>
-      <c s="19"/>
-      <c s="3" t="s">
-        <v>73</v>
-      </c>
-      <c s="3" t="s">
-        <v>77</v>
-      </c>
-      <c s="3"/>
-      <c s="3"/>
-      <c s="3"/>
-    </row>
-    <row>
-      <c s="3"/>
-      <c s="19"/>
+      <c s="15"/>
+      <c s="3" t="s">
+        <v>74</v>
+      </c>
+      <c s="3" t="s">
+        <v>78</v>
+      </c>
+      <c s="3"/>
+      <c s="3"/>
+      <c s="3"/>
+    </row>
+    <row>
+      <c s="3"/>
+      <c s="15"/>
       <c s="3" t="s">
         <v>7</v>
       </c>
@@ -1722,87 +1729,87 @@
     </row>
     <row>
       <c s="3"/>
-      <c s="19"/>
+      <c s="15"/>
       <c s="3" t="s">
         <v>32</v>
       </c>
       <c s="3" t="s">
+        <v>19</v>
+      </c>
+      <c s="3"/>
+      <c s="3" t="s">
+        <v>42</v>
+      </c>
+      <c s="3"/>
+    </row>
+    <row>
+      <c s="3"/>
+      <c s="15"/>
+      <c s="3" t="s">
+        <v>60</v>
+      </c>
+      <c s="1" t="s">
+        <v>62</v>
+      </c>
+      <c s="3"/>
+      <c s="3" t="s">
+        <v>26</v>
+      </c>
+      <c s="3"/>
+    </row>
+    <row>
+      <c s="3"/>
+      <c s="15"/>
+      <c s="3" t="s">
+        <v>87</v>
+      </c>
+      <c s="3" t="s">
+        <v>6</v>
+      </c>
+      <c s="3"/>
+      <c s="3"/>
+      <c s="3"/>
+    </row>
+    <row>
+      <c s="3" t="s">
+        <v>35</v>
+      </c>
+      <c s="15" t="s">
+        <v>48</v>
+      </c>
+      <c s="3" t="s">
+        <v>67</v>
+      </c>
+      <c s="3" t="s">
+        <v>30</v>
+      </c>
+      <c s="3" t="s">
+        <v>35</v>
+      </c>
+      <c s="3"/>
+      <c s="3"/>
+    </row>
+    <row>
+      <c s="3"/>
+      <c s="15"/>
+      <c s="3" t="s">
+        <v>88</v>
+      </c>
+      <c s="1" t="s">
+        <v>4</v>
+      </c>
+      <c s="17"/>
+      <c s="3" t="s">
+        <v>68</v>
+      </c>
+      <c s="3"/>
+    </row>
+    <row>
+      <c s="3"/>
+      <c s="15"/>
+      <c s="3" t="s">
         <v>20</v>
       </c>
-      <c s="3"/>
-      <c s="3" t="s">
-        <v>42</v>
-      </c>
-      <c s="3"/>
-    </row>
-    <row>
-      <c s="3"/>
-      <c s="19"/>
-      <c s="3" t="s">
-        <v>60</v>
-      </c>
-      <c s="1" t="s">
-        <v>62</v>
-      </c>
-      <c s="3"/>
-      <c s="3" t="s">
-        <v>27</v>
-      </c>
-      <c s="3"/>
-    </row>
-    <row>
-      <c s="3"/>
-      <c s="19"/>
-      <c s="3" t="s">
-        <v>85</v>
-      </c>
-      <c s="3" t="s">
-        <v>6</v>
-      </c>
-      <c s="3"/>
-      <c s="3"/>
-      <c s="3"/>
-    </row>
-    <row>
-      <c s="3" t="s">
-        <v>35</v>
-      </c>
-      <c s="19" t="s">
-        <v>48</v>
-      </c>
-      <c s="3" t="s">
-        <v>67</v>
-      </c>
-      <c s="3" t="s">
-        <v>30</v>
-      </c>
-      <c s="3" t="s">
-        <v>35</v>
-      </c>
-      <c s="3"/>
-      <c s="3"/>
-    </row>
-    <row>
-      <c s="3"/>
-      <c s="19"/>
-      <c s="3" t="s">
-        <v>86</v>
-      </c>
-      <c s="1" t="s">
-        <v>4</v>
-      </c>
-      <c s="21"/>
-      <c s="3" t="s">
-        <v>68</v>
-      </c>
-      <c s="3"/>
-    </row>
-    <row>
-      <c s="3"/>
-      <c s="19"/>
-      <c s="3" t="s">
-        <v>21</v>
-      </c>
       <c s="3" t="s">
         <v>66</v>
       </c>
@@ -1810,12 +1817,12 @@
       <c s="3"/>
       <c s="3"/>
     </row>
-    <row>
+    <row ht="14.4" customHeight="1">
       <c s="7" t="s">
         <v>57</v>
       </c>
       <c s="7" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c s="2" t="s">
         <v>67</v>
@@ -1833,8 +1840,55 @@
       <c s="7"/>
       <c s="7"/>
       <c s="2" t="s">
+        <v>88</v>
+      </c>
+      <c s="1" t="s">
+        <v>4</v>
+      </c>
+      <c s="2"/>
+      <c s="2" t="s">
+        <v>68</v>
+      </c>
+      <c s="2"/>
+    </row>
+    <row>
+      <c s="7"/>
+      <c s="7"/>
+      <c s="2" t="s">
+        <v>20</v>
+      </c>
+      <c s="1" t="s">
+        <v>71</v>
+      </c>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+    </row>
+    <row>
+      <c s="7" t="s">
         <v>86</v>
       </c>
+      <c s="7" t="s">
+        <v>28</v>
+      </c>
+      <c s="2" t="s">
+        <v>67</v>
+      </c>
+      <c s="2" t="s">
+        <v>30</v>
+      </c>
+      <c s="2" t="s">
+        <v>86</v>
+      </c>
+      <c s="2"/>
+      <c s="2"/>
+    </row>
+    <row>
+      <c s="7"/>
+      <c s="7"/>
+      <c s="2" t="s">
+        <v>88</v>
+      </c>
       <c s="1" t="s">
         <v>4</v>
       </c>
@@ -1848,17 +1902,17 @@
       <c s="7"/>
       <c s="7"/>
       <c s="2" t="s">
-        <v>21</v>
-      </c>
-      <c s="1" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c s="1" t="s">
+        <v>71</v>
       </c>
       <c s="1"/>
       <c s="1"/>
       <c s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="26">
     <mergeCell ref="A2:A6"/>
     <mergeCell ref="B2:B6"/>
     <mergeCell ref="A7:A9"/>
@@ -1883,6 +1937,8 @@
     <mergeCell ref="B58:B60"/>
     <mergeCell ref="A61:A63"/>
     <mergeCell ref="B61:B63"/>
+    <mergeCell ref="A64:A66"/>
+    <mergeCell ref="B64:B66"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200"/>
@@ -1891,20 +1947,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G63"/>
+  <dimension ref="A1:G66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A63" sqref="A61:G63"/>
+      <selection activeCell="A66" sqref="A64:G66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" style="24" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.6640625" style="26" customWidth="1"/>
-    <col min="3" max="3" width="9.078125" style="24" customWidth="1"/>
-    <col min="4" max="4" width="28" style="24" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="19" style="24" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.078125" style="24" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" style="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.6640625" style="25" customWidth="1"/>
+    <col min="3" max="3" width="9.078125" style="26" customWidth="1"/>
+    <col min="4" max="4" width="28" style="26" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19" style="26" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="38.21875" style="26" customWidth="1"/>
+    <col min="7" max="16384" width="9.078125" style="26" customWidth="1"/>
   </cols>
   <sheetData>
     <row ht="15.1" customFormat="1">
@@ -1918,10 +1975,10 @@
         <v>0</v>
       </c>
       <c t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c t="s">
         <v>36</v>
@@ -1931,8 +1988,8 @@
       </c>
     </row>
     <row>
-      <c s="23" t="s">
-        <v>79</v>
+      <c s="24" t="s">
+        <v>80</v>
       </c>
       <c s="6" t="s">
         <v>58</v>
@@ -1944,81 +2001,389 @@
         <v>30</v>
       </c>
       <c s="5" t="s">
+        <v>80</v>
+      </c>
+      <c s="5"/>
+      <c s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row>
+      <c s="24"/>
+      <c s="6"/>
+      <c s="5" t="s">
+        <v>88</v>
+      </c>
+      <c s="5" t="s">
+        <v>38</v>
+      </c>
+      <c s="5"/>
+      <c s="5"/>
+      <c s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row>
+      <c s="24"/>
+      <c s="6"/>
+      <c s="5" t="s">
+        <v>20</v>
+      </c>
+      <c s="5" t="s">
+        <v>14</v>
+      </c>
+      <c s="5"/>
+      <c s="5"/>
+      <c s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row>
+      <c s="24"/>
+      <c s="6"/>
+      <c s="5" t="s">
+        <v>43</v>
+      </c>
+      <c s="5" t="s">
         <v>79</v>
       </c>
       <c s="5"/>
-      <c s="14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row>
-      <c s="23"/>
+      <c s="5" t="s">
+        <v>68</v>
+      </c>
+      <c s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row>
+      <c s="24"/>
       <c s="6"/>
       <c s="5" t="s">
-        <v>86</v>
-      </c>
-      <c s="5" t="s">
-        <v>38</v>
-      </c>
-      <c s="5"/>
-      <c s="5"/>
-      <c s="14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row>
-      <c s="23"/>
-      <c s="6"/>
-      <c s="5" t="s">
-        <v>21</v>
-      </c>
-      <c s="5" t="s">
+        <v>69</v>
+      </c>
+      <c s="5" t="s">
+        <v>23</v>
+      </c>
+      <c s="5"/>
+      <c s="5"/>
+      <c s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row>
+      <c s="24" t="s">
+        <v>31</v>
+      </c>
+      <c s="11" t="s">
+        <v>3</v>
+      </c>
+      <c s="5" t="s">
+        <v>67</v>
+      </c>
+      <c s="5" t="s">
+        <v>30</v>
+      </c>
+      <c s="5" t="s">
+        <v>31</v>
+      </c>
+      <c s="5"/>
+      <c s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row>
+      <c s="24"/>
+      <c s="11"/>
+      <c s="5" t="s">
+        <v>88</v>
+      </c>
+      <c s="5" t="s">
+        <v>4</v>
+      </c>
+      <c s="5"/>
+      <c s="5" t="s">
+        <v>68</v>
+      </c>
+      <c s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row>
+      <c s="24"/>
+      <c s="11"/>
+      <c s="5" t="s">
+        <v>20</v>
+      </c>
+      <c s="5" t="s">
+        <v>23</v>
+      </c>
+      <c s="5"/>
+      <c s="5"/>
+      <c s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row>
+      <c s="24" t="s">
+        <v>53</v>
+      </c>
+      <c s="11" t="s">
+        <v>92</v>
+      </c>
+      <c s="5" t="s">
+        <v>67</v>
+      </c>
+      <c s="5" t="s">
+        <v>30</v>
+      </c>
+      <c s="5" t="s">
+        <v>53</v>
+      </c>
+      <c s="5"/>
+      <c s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row>
+      <c s="24"/>
+      <c s="11"/>
+      <c s="5" t="s">
+        <v>88</v>
+      </c>
+      <c s="5" t="s">
+        <v>4</v>
+      </c>
+      <c s="5"/>
+      <c s="5" t="s">
+        <v>68</v>
+      </c>
+      <c s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row>
+      <c s="24"/>
+      <c s="11"/>
+      <c s="5" t="s">
+        <v>20</v>
+      </c>
+      <c s="5" t="s">
+        <v>23</v>
+      </c>
+      <c s="5"/>
+      <c s="5"/>
+      <c s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row>
+      <c s="24" t="s">
+        <v>81</v>
+      </c>
+      <c s="11" t="s">
         <v>15</v>
       </c>
-      <c s="5"/>
-      <c s="5"/>
-      <c s="14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row>
-      <c s="23"/>
-      <c s="6"/>
+      <c s="5" t="s">
+        <v>67</v>
+      </c>
+      <c s="5" t="s">
+        <v>30</v>
+      </c>
+      <c s="5" t="s">
+        <v>81</v>
+      </c>
+      <c s="5"/>
+      <c s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row>
+      <c s="24"/>
+      <c s="11"/>
+      <c s="5" t="s">
+        <v>88</v>
+      </c>
+      <c s="5" t="s">
+        <v>4</v>
+      </c>
+      <c s="5"/>
+      <c s="5" t="s">
+        <v>68</v>
+      </c>
+      <c s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row>
+      <c s="24"/>
+      <c s="11"/>
+      <c s="5" t="s">
+        <v>20</v>
+      </c>
+      <c s="5" t="s">
+        <v>23</v>
+      </c>
+      <c s="5"/>
+      <c s="5"/>
+      <c s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row>
+      <c s="24"/>
+      <c s="11"/>
       <c s="5" t="s">
         <v>43</v>
       </c>
       <c s="5" t="s">
-        <v>78</v>
+        <v>62</v>
+      </c>
+      <c s="5"/>
+      <c s="5" t="s">
+        <v>2</v>
+      </c>
+      <c s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row>
+      <c s="24"/>
+      <c s="11"/>
+      <c s="5" t="s">
+        <v>69</v>
+      </c>
+      <c s="5" t="s">
+        <v>59</v>
+      </c>
+      <c s="5"/>
+      <c s="5"/>
+      <c s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row>
+      <c s="24" t="s">
+        <v>8</v>
+      </c>
+      <c s="11" t="s">
+        <v>24</v>
+      </c>
+      <c s="5" t="s">
+        <v>67</v>
+      </c>
+      <c s="5" t="s">
+        <v>30</v>
+      </c>
+      <c s="5" t="s">
+        <v>8</v>
+      </c>
+      <c s="5"/>
+      <c s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row>
+      <c s="24"/>
+      <c s="11"/>
+      <c s="5" t="s">
+        <v>88</v>
+      </c>
+      <c s="5" t="s">
+        <v>4</v>
       </c>
       <c s="5"/>
       <c s="5" t="s">
         <v>68</v>
       </c>
-      <c s="14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row>
-      <c s="23"/>
-      <c s="6"/>
+      <c s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row>
+      <c s="24"/>
+      <c s="11"/>
+      <c s="5" t="s">
+        <v>20</v>
+      </c>
+      <c s="5" t="s">
+        <v>23</v>
+      </c>
+      <c s="5"/>
+      <c s="5"/>
+      <c s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row>
+      <c s="24"/>
+      <c s="11"/>
+      <c s="5" t="s">
+        <v>43</v>
+      </c>
+      <c s="5" t="s">
+        <v>62</v>
+      </c>
+      <c s="5"/>
+      <c s="5" t="s">
+        <v>2</v>
+      </c>
+      <c s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row>
+      <c s="24"/>
+      <c s="11"/>
       <c s="5" t="s">
         <v>69</v>
       </c>
       <c s="5" t="s">
-        <v>24</v>
-      </c>
-      <c s="5"/>
-      <c s="5"/>
-      <c s="14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row>
-      <c s="23" t="s">
-        <v>31</v>
-      </c>
-      <c s="8" t="s">
-        <v>3</v>
+        <v>59</v>
+      </c>
+      <c s="5"/>
+      <c s="5"/>
+      <c s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row>
+      <c s="24"/>
+      <c s="11"/>
+      <c s="5" t="s">
+        <v>91</v>
+      </c>
+      <c s="5" t="s">
+        <v>62</v>
+      </c>
+      <c s="5"/>
+      <c s="5" t="s">
+        <v>26</v>
+      </c>
+      <c s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row>
+      <c s="24"/>
+      <c s="11"/>
+      <c s="5" t="s">
+        <v>25</v>
+      </c>
+      <c s="5" t="s">
+        <v>75</v>
+      </c>
+      <c s="5"/>
+      <c s="5"/>
+      <c s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row ht="15" customHeight="1">
+      <c s="11" t="s">
+        <v>54</v>
+      </c>
+      <c s="11" t="s">
+        <v>39</v>
       </c>
       <c s="5" t="s">
         <v>67</v>
@@ -2027,18 +2392,18 @@
         <v>30</v>
       </c>
       <c s="5" t="s">
-        <v>31</v>
-      </c>
-      <c s="5"/>
-      <c s="14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row>
-      <c s="23"/>
-      <c s="8"/>
-      <c s="5" t="s">
-        <v>86</v>
+        <v>54</v>
+      </c>
+      <c s="5"/>
+      <c s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row>
+      <c s="11"/>
+      <c s="11"/>
+      <c s="5" t="s">
+        <v>88</v>
       </c>
       <c s="5" t="s">
         <v>4</v>
@@ -2047,31 +2412,95 @@
       <c s="5" t="s">
         <v>68</v>
       </c>
-      <c s="14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row>
-      <c s="23"/>
-      <c s="8"/>
-      <c s="5" t="s">
-        <v>21</v>
-      </c>
-      <c s="5" t="s">
-        <v>24</v>
-      </c>
-      <c s="5"/>
-      <c s="5"/>
-      <c s="14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row>
-      <c s="23" t="s">
-        <v>53</v>
-      </c>
-      <c s="8" t="s">
-        <v>90</v>
+      <c s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row>
+      <c s="11"/>
+      <c s="11"/>
+      <c s="5" t="s">
+        <v>20</v>
+      </c>
+      <c s="5" t="s">
+        <v>23</v>
+      </c>
+      <c s="5"/>
+      <c s="5"/>
+      <c s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row>
+      <c s="11"/>
+      <c s="11"/>
+      <c s="5" t="s">
+        <v>43</v>
+      </c>
+      <c s="5" t="s">
+        <v>62</v>
+      </c>
+      <c s="5"/>
+      <c s="5" t="s">
+        <v>2</v>
+      </c>
+      <c s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row>
+      <c s="11"/>
+      <c s="11"/>
+      <c s="5" t="s">
+        <v>69</v>
+      </c>
+      <c s="5" t="s">
+        <v>59</v>
+      </c>
+      <c s="5"/>
+      <c s="5"/>
+      <c s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row>
+      <c s="11"/>
+      <c s="11"/>
+      <c s="5" t="s">
+        <v>91</v>
+      </c>
+      <c s="5" t="s">
+        <v>62</v>
+      </c>
+      <c s="5"/>
+      <c s="5" t="s">
+        <v>26</v>
+      </c>
+      <c s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row>
+      <c s="11"/>
+      <c s="11"/>
+      <c s="5" t="s">
+        <v>25</v>
+      </c>
+      <c s="5" t="s">
+        <v>50</v>
+      </c>
+      <c s="5"/>
+      <c s="5"/>
+      <c s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row>
+      <c s="11" t="s">
+        <v>5</v>
+      </c>
+      <c s="11" t="s">
+        <v>41</v>
       </c>
       <c s="5" t="s">
         <v>67</v>
@@ -2080,18 +2509,18 @@
         <v>30</v>
       </c>
       <c s="5" t="s">
-        <v>53</v>
-      </c>
-      <c s="5"/>
-      <c s="14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row>
-      <c s="23"/>
-      <c s="8"/>
-      <c s="5" t="s">
-        <v>86</v>
+        <v>5</v>
+      </c>
+      <c s="5"/>
+      <c s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row>
+      <c s="11"/>
+      <c s="11"/>
+      <c s="5" t="s">
+        <v>88</v>
       </c>
       <c s="5" t="s">
         <v>4</v>
@@ -2100,31 +2529,95 @@
       <c s="5" t="s">
         <v>68</v>
       </c>
-      <c s="14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row>
-      <c s="23"/>
-      <c s="8"/>
-      <c s="5" t="s">
-        <v>21</v>
-      </c>
-      <c s="5" t="s">
-        <v>24</v>
-      </c>
-      <c s="5"/>
-      <c s="5"/>
-      <c s="14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row>
-      <c s="23" t="s">
-        <v>80</v>
-      </c>
-      <c s="8" t="s">
-        <v>16</v>
+      <c s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row>
+      <c s="11"/>
+      <c s="11"/>
+      <c s="5" t="s">
+        <v>20</v>
+      </c>
+      <c s="5" t="s">
+        <v>23</v>
+      </c>
+      <c s="5"/>
+      <c s="5"/>
+      <c s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row>
+      <c s="11"/>
+      <c s="11"/>
+      <c s="5" t="s">
+        <v>43</v>
+      </c>
+      <c s="5" t="s">
+        <v>62</v>
+      </c>
+      <c s="5"/>
+      <c s="5" t="s">
+        <v>2</v>
+      </c>
+      <c s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row>
+      <c s="11"/>
+      <c s="11"/>
+      <c s="5" t="s">
+        <v>69</v>
+      </c>
+      <c s="5" t="s">
+        <v>59</v>
+      </c>
+      <c s="5"/>
+      <c s="5"/>
+      <c s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row>
+      <c s="11"/>
+      <c s="11"/>
+      <c s="5" t="s">
+        <v>91</v>
+      </c>
+      <c s="5" t="s">
+        <v>62</v>
+      </c>
+      <c s="5"/>
+      <c s="5" t="s">
+        <v>26</v>
+      </c>
+      <c s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row>
+      <c s="11"/>
+      <c s="11"/>
+      <c s="5" t="s">
+        <v>25</v>
+      </c>
+      <c s="5" t="s">
+        <v>17</v>
+      </c>
+      <c s="5"/>
+      <c s="5"/>
+      <c s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row>
+      <c s="11" t="s">
+        <v>34</v>
+      </c>
+      <c s="11" t="s">
+        <v>63</v>
       </c>
       <c s="5" t="s">
         <v>67</v>
@@ -2133,18 +2626,18 @@
         <v>30</v>
       </c>
       <c s="5" t="s">
-        <v>80</v>
-      </c>
-      <c s="5"/>
-      <c s="14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row>
-      <c s="23"/>
-      <c s="8"/>
-      <c s="5" t="s">
-        <v>86</v>
+        <v>34</v>
+      </c>
+      <c s="5"/>
+      <c s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row>
+      <c s="11"/>
+      <c s="11"/>
+      <c s="5" t="s">
+        <v>88</v>
       </c>
       <c s="5" t="s">
         <v>4</v>
@@ -2153,63 +2646,31 @@
       <c s="5" t="s">
         <v>68</v>
       </c>
-      <c s="14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row>
-      <c s="23"/>
-      <c s="8"/>
-      <c s="5" t="s">
-        <v>21</v>
-      </c>
-      <c s="5" t="s">
-        <v>24</v>
-      </c>
-      <c s="5"/>
-      <c s="5"/>
-      <c s="14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row>
-      <c s="23"/>
-      <c s="8"/>
-      <c s="5" t="s">
-        <v>43</v>
-      </c>
-      <c s="5" t="s">
-        <v>62</v>
-      </c>
-      <c s="5"/>
-      <c s="5" t="s">
-        <v>2</v>
-      </c>
-      <c s="14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row>
-      <c s="23"/>
-      <c s="8"/>
-      <c s="5" t="s">
-        <v>69</v>
-      </c>
-      <c s="5" t="s">
-        <v>59</v>
-      </c>
-      <c s="5"/>
-      <c s="5"/>
-      <c s="14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row>
-      <c s="23" t="s">
-        <v>8</v>
-      </c>
-      <c s="8" t="s">
-        <v>25</v>
+      <c s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row>
+      <c s="11"/>
+      <c s="11"/>
+      <c s="5" t="s">
+        <v>20</v>
+      </c>
+      <c s="5" t="s">
+        <v>47</v>
+      </c>
+      <c s="5"/>
+      <c s="5"/>
+      <c s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row>
+      <c s="11" t="s">
+        <v>56</v>
+      </c>
+      <c s="11" t="s">
+        <v>9</v>
       </c>
       <c s="5" t="s">
         <v>67</v>
@@ -2218,18 +2679,18 @@
         <v>30</v>
       </c>
       <c s="5" t="s">
-        <v>8</v>
-      </c>
-      <c s="5"/>
-      <c s="14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row>
-      <c s="23"/>
-      <c s="8"/>
-      <c s="5" t="s">
-        <v>86</v>
+        <v>56</v>
+      </c>
+      <c s="5"/>
+      <c s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row>
+      <c s="11"/>
+      <c s="11"/>
+      <c s="5" t="s">
+        <v>88</v>
       </c>
       <c s="5" t="s">
         <v>4</v>
@@ -2238,426 +2699,22 @@
       <c s="5" t="s">
         <v>68</v>
       </c>
-      <c s="14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row>
-      <c s="23"/>
-      <c s="8"/>
-      <c s="5" t="s">
-        <v>21</v>
-      </c>
-      <c s="5" t="s">
-        <v>24</v>
-      </c>
-      <c s="5"/>
-      <c s="5"/>
-      <c s="14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row>
-      <c s="23"/>
-      <c s="8"/>
-      <c s="5" t="s">
-        <v>43</v>
-      </c>
-      <c s="5" t="s">
-        <v>62</v>
-      </c>
-      <c s="5"/>
-      <c s="5" t="s">
-        <v>2</v>
-      </c>
-      <c s="14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row>
-      <c s="23"/>
-      <c s="8"/>
-      <c s="5" t="s">
-        <v>69</v>
-      </c>
-      <c s="5" t="s">
-        <v>59</v>
-      </c>
-      <c s="5"/>
-      <c s="5"/>
-      <c s="14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row>
-      <c s="23"/>
-      <c s="8"/>
-      <c s="5" t="s">
-        <v>89</v>
-      </c>
-      <c s="5" t="s">
-        <v>62</v>
-      </c>
-      <c s="5"/>
-      <c s="5" t="s">
-        <v>27</v>
-      </c>
-      <c s="14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row>
-      <c s="23"/>
-      <c s="8"/>
-      <c s="5" t="s">
-        <v>26</v>
-      </c>
-      <c s="5" t="s">
-        <v>74</v>
-      </c>
-      <c s="5"/>
-      <c s="5"/>
-      <c s="14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row ht="15" customHeight="1">
-      <c s="8" t="s">
-        <v>54</v>
-      </c>
-      <c s="8" t="s">
-        <v>39</v>
-      </c>
-      <c s="5" t="s">
-        <v>67</v>
-      </c>
-      <c s="5" t="s">
-        <v>30</v>
-      </c>
-      <c s="5" t="s">
-        <v>54</v>
-      </c>
-      <c s="5"/>
-      <c s="14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row>
-      <c s="8"/>
-      <c s="8"/>
-      <c s="5" t="s">
-        <v>86</v>
-      </c>
-      <c s="5" t="s">
-        <v>4</v>
-      </c>
-      <c s="5"/>
-      <c s="5" t="s">
-        <v>68</v>
-      </c>
-      <c s="14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row>
-      <c s="8"/>
-      <c s="8"/>
-      <c s="5" t="s">
-        <v>21</v>
-      </c>
-      <c s="5" t="s">
-        <v>24</v>
-      </c>
-      <c s="5"/>
-      <c s="5"/>
-      <c s="14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row>
-      <c s="8"/>
-      <c s="8"/>
-      <c s="5" t="s">
-        <v>43</v>
-      </c>
-      <c s="5" t="s">
-        <v>62</v>
-      </c>
-      <c s="5"/>
-      <c s="5" t="s">
-        <v>2</v>
-      </c>
-      <c s="14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row>
-      <c s="8"/>
-      <c s="8"/>
-      <c s="5" t="s">
-        <v>69</v>
-      </c>
-      <c s="5" t="s">
-        <v>59</v>
-      </c>
-      <c s="5"/>
-      <c s="5"/>
-      <c s="14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row>
-      <c s="8"/>
-      <c s="8"/>
-      <c s="5" t="s">
-        <v>89</v>
-      </c>
-      <c s="5" t="s">
-        <v>62</v>
-      </c>
-      <c s="5"/>
-      <c s="5" t="s">
-        <v>27</v>
-      </c>
-      <c s="14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row>
-      <c s="8"/>
-      <c s="8"/>
-      <c s="5" t="s">
-        <v>26</v>
-      </c>
-      <c s="5" t="s">
-        <v>50</v>
-      </c>
-      <c s="5"/>
-      <c s="5"/>
-      <c s="14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row>
-      <c s="8" t="s">
-        <v>5</v>
-      </c>
-      <c s="8" t="s">
-        <v>41</v>
-      </c>
-      <c s="5" t="s">
-        <v>67</v>
-      </c>
-      <c s="5" t="s">
-        <v>30</v>
-      </c>
-      <c s="5" t="s">
-        <v>5</v>
-      </c>
-      <c s="5"/>
-      <c s="14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row>
-      <c s="8"/>
-      <c s="8"/>
-      <c s="5" t="s">
-        <v>86</v>
-      </c>
-      <c s="5" t="s">
-        <v>4</v>
-      </c>
-      <c s="5"/>
-      <c s="5" t="s">
-        <v>68</v>
-      </c>
-      <c s="14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row>
-      <c s="8"/>
-      <c s="8"/>
-      <c s="5" t="s">
-        <v>21</v>
-      </c>
-      <c s="5" t="s">
-        <v>24</v>
-      </c>
-      <c s="5"/>
-      <c s="5"/>
-      <c s="14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row>
-      <c s="8"/>
-      <c s="8"/>
-      <c s="5" t="s">
-        <v>43</v>
-      </c>
-      <c s="5" t="s">
-        <v>62</v>
-      </c>
-      <c s="5"/>
-      <c s="5" t="s">
-        <v>2</v>
-      </c>
-      <c s="14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row>
-      <c s="8"/>
-      <c s="8"/>
-      <c s="5" t="s">
-        <v>69</v>
-      </c>
-      <c s="5" t="s">
-        <v>59</v>
-      </c>
-      <c s="5"/>
-      <c s="5"/>
-      <c s="14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row>
-      <c s="8"/>
-      <c s="8"/>
-      <c s="5" t="s">
-        <v>89</v>
-      </c>
-      <c s="5" t="s">
-        <v>62</v>
-      </c>
-      <c s="5"/>
-      <c s="5" t="s">
-        <v>27</v>
-      </c>
-      <c s="14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row>
-      <c s="8"/>
-      <c s="8"/>
-      <c s="5" t="s">
-        <v>26</v>
-      </c>
-      <c s="5" t="s">
-        <v>18</v>
-      </c>
-      <c s="5"/>
-      <c s="5"/>
-      <c s="14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row>
-      <c s="8" t="s">
-        <v>34</v>
-      </c>
-      <c s="8" t="s">
-        <v>63</v>
-      </c>
-      <c s="5" t="s">
-        <v>67</v>
-      </c>
-      <c s="5" t="s">
-        <v>30</v>
-      </c>
-      <c s="5" t="s">
-        <v>34</v>
-      </c>
-      <c s="5"/>
-      <c s="14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row>
-      <c s="8"/>
-      <c s="8"/>
-      <c s="5" t="s">
-        <v>86</v>
-      </c>
-      <c s="5" t="s">
-        <v>4</v>
-      </c>
-      <c s="5"/>
-      <c s="5" t="s">
-        <v>68</v>
-      </c>
-      <c s="14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row>
-      <c s="8"/>
-      <c s="8"/>
-      <c s="5" t="s">
-        <v>21</v>
+      <c s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row>
+      <c s="11"/>
+      <c s="11"/>
+      <c s="5" t="s">
+        <v>20</v>
       </c>
       <c s="5" t="s">
         <v>47</v>
       </c>
       <c s="5"/>
       <c s="5"/>
-      <c s="14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row>
-      <c s="8" t="s">
-        <v>56</v>
-      </c>
-      <c s="8" t="s">
-        <v>9</v>
-      </c>
-      <c s="5" t="s">
-        <v>67</v>
-      </c>
-      <c s="5" t="s">
-        <v>30</v>
-      </c>
-      <c s="5" t="s">
-        <v>56</v>
-      </c>
-      <c s="5"/>
-      <c s="14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row>
-      <c s="8"/>
-      <c s="8"/>
-      <c s="5" t="s">
-        <v>86</v>
-      </c>
-      <c s="5" t="s">
-        <v>4</v>
-      </c>
-      <c s="5"/>
-      <c s="5" t="s">
-        <v>68</v>
-      </c>
-      <c s="14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row>
-      <c s="8"/>
-      <c s="8"/>
-      <c s="5" t="s">
-        <v>21</v>
-      </c>
-      <c s="5" t="s">
-        <v>47</v>
-      </c>
-      <c s="5"/>
-      <c s="5"/>
-      <c s="14" t="s">
+      <c s="19" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2678,15 +2735,15 @@
         <v>10</v>
       </c>
       <c s="6"/>
-      <c s="25" t="s">
-        <v>84</v>
+      <c s="23" t="s">
+        <v>11</v>
       </c>
     </row>
     <row>
       <c s="6"/>
       <c s="27"/>
       <c s="6" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c s="5" t="s">
         <v>4</v>
@@ -2695,24 +2752,24 @@
       <c s="6" t="s">
         <v>68</v>
       </c>
-      <c s="25" t="s">
-        <v>12</v>
+      <c s="23" t="s">
+        <v>11</v>
       </c>
     </row>
     <row>
       <c s="6"/>
       <c s="27"/>
       <c s="6" t="s">
-        <v>21</v>
-      </c>
-      <c s="5" t="s">
         <v>20</v>
+      </c>
+      <c s="5" t="s">
+        <v>19</v>
       </c>
       <c s="5"/>
       <c s="6" t="s">
         <v>65</v>
       </c>
-      <c s="25" t="s">
+      <c s="23" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2729,7 +2786,7 @@
       <c s="6" t="s">
         <v>2</v>
       </c>
-      <c s="25" t="s">
+      <c s="23" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2740,11 +2797,11 @@
         <v>69</v>
       </c>
       <c s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c s="6"/>
       <c s="5"/>
-      <c s="25" t="s">
+      <c s="23" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2752,16 +2809,16 @@
       <c s="6"/>
       <c s="27"/>
       <c s="6" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c s="5" t="s">
         <v>62</v>
       </c>
       <c s="6"/>
       <c s="6" t="s">
-        <v>27</v>
-      </c>
-      <c s="25" t="s">
+        <v>26</v>
+      </c>
+      <c s="23" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2769,14 +2826,14 @@
       <c s="6"/>
       <c s="27"/>
       <c s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c s="5" t="s">
         <v>59</v>
       </c>
       <c s="6"/>
       <c s="6"/>
-      <c s="25" t="s">
+      <c s="23" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2793,7 +2850,7 @@
       <c s="6" t="s">
         <v>2</v>
       </c>
-      <c s="25" t="s">
+      <c s="23" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2801,14 +2858,14 @@
       <c s="6"/>
       <c s="27"/>
       <c s="6" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c s="6" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c s="6"/>
       <c s="6"/>
-      <c s="25" t="s">
+      <c s="23" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2825,7 +2882,7 @@
       <c s="6" t="s">
         <v>68</v>
       </c>
-      <c s="25" t="s">
+      <c s="23" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2836,13 +2893,13 @@
         <v>32</v>
       </c>
       <c s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c s="6"/>
       <c s="6" t="s">
         <v>42</v>
       </c>
-      <c s="25" t="s">
+      <c s="23" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2857,9 +2914,9 @@
       </c>
       <c s="6"/>
       <c s="6" t="s">
-        <v>27</v>
-      </c>
-      <c s="25" t="s">
+        <v>26</v>
+      </c>
+      <c s="23" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2867,14 +2924,14 @@
       <c s="6"/>
       <c s="27"/>
       <c s="6" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c s="6" t="s">
         <v>6</v>
       </c>
       <c s="6"/>
       <c s="6"/>
-      <c s="25" t="s">
+      <c s="23" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2895,15 +2952,15 @@
         <v>35</v>
       </c>
       <c s="6"/>
-      <c s="25" t="s">
-        <v>84</v>
+      <c s="23" t="s">
+        <v>11</v>
       </c>
     </row>
     <row>
       <c s="6"/>
       <c s="27"/>
       <c s="6" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c s="5" t="s">
         <v>4</v>
@@ -2912,31 +2969,31 @@
       <c s="6" t="s">
         <v>68</v>
       </c>
-      <c s="25" t="s">
-        <v>84</v>
+      <c s="23" t="s">
+        <v>11</v>
       </c>
     </row>
     <row>
       <c s="6"/>
       <c s="27"/>
       <c s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c s="6" t="s">
         <v>66</v>
       </c>
       <c s="6"/>
       <c s="6"/>
-      <c s="25" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row>
-      <c s="8" t="s">
+      <c s="23" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row ht="14.4" customHeight="1">
+      <c s="11" t="s">
         <v>57</v>
       </c>
-      <c s="8" t="s">
-        <v>83</v>
+      <c s="11" t="s">
+        <v>84</v>
       </c>
       <c s="5" t="s">
         <v>67</v>
@@ -2948,16 +3005,69 @@
         <v>57</v>
       </c>
       <c s="5"/>
-      <c s="14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row>
-      <c s="8"/>
-      <c s="8"/>
-      <c s="5" t="s">
+      <c s="19" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row>
+      <c s="11"/>
+      <c s="11"/>
+      <c s="5" t="s">
+        <v>88</v>
+      </c>
+      <c s="5" t="s">
+        <v>4</v>
+      </c>
+      <c s="5"/>
+      <c s="5" t="s">
+        <v>68</v>
+      </c>
+      <c s="19" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row>
+      <c s="11"/>
+      <c s="11"/>
+      <c s="5" t="s">
+        <v>20</v>
+      </c>
+      <c s="5" t="s">
+        <v>71</v>
+      </c>
+      <c s="5"/>
+      <c s="5"/>
+      <c s="19" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row>
+      <c s="11" t="s">
         <v>86</v>
       </c>
+      <c s="11" t="s">
+        <v>28</v>
+      </c>
+      <c s="5" t="s">
+        <v>67</v>
+      </c>
+      <c s="5" t="s">
+        <v>30</v>
+      </c>
+      <c s="5" t="s">
+        <v>86</v>
+      </c>
+      <c s="5"/>
+      <c s="19" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row>
+      <c s="11"/>
+      <c s="11"/>
+      <c s="5" t="s">
+        <v>88</v>
+      </c>
       <c s="5" t="s">
         <v>4</v>
       </c>
@@ -2965,27 +3075,27 @@
       <c s="5" t="s">
         <v>68</v>
       </c>
-      <c s="14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row>
-      <c s="8"/>
-      <c s="8"/>
-      <c s="5" t="s">
-        <v>21</v>
-      </c>
-      <c s="5" t="s">
-        <v>19</v>
-      </c>
-      <c s="5"/>
-      <c s="5"/>
-      <c s="14" t="s">
-        <v>11</v>
+      <c s="19" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row>
+      <c s="11"/>
+      <c s="11"/>
+      <c s="5" t="s">
+        <v>20</v>
+      </c>
+      <c s="5" t="s">
+        <v>71</v>
+      </c>
+      <c s="5"/>
+      <c s="5"/>
+      <c s="19" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="26">
     <mergeCell ref="A2:A6"/>
     <mergeCell ref="B2:B6"/>
     <mergeCell ref="A7:A9"/>
@@ -3010,6 +3120,8 @@
     <mergeCell ref="B58:B60"/>
     <mergeCell ref="A61:A63"/>
     <mergeCell ref="B61:B63"/>
+    <mergeCell ref="A64:A66"/>
+    <mergeCell ref="B64:B66"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200"/>
@@ -3044,10 +3156,10 @@
         <v>0</v>
       </c>
       <c s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c s="4" t="s">
         <v>36</v>
@@ -3057,11 +3169,11 @@
       </c>
     </row>
     <row>
-      <c s="20" t="s">
+      <c s="14" t="s">
         <v>33</v>
       </c>
-      <c s="20" t="s">
-        <v>75</v>
+      <c s="14" t="s">
+        <v>76</v>
       </c>
       <c s="2" t="s">
         <v>67</v>
@@ -3076,10 +3188,10 @@
       <c s="1"/>
     </row>
     <row>
-      <c s="20"/>
-      <c s="20"/>
-      <c s="2" t="s">
-        <v>86</v>
+      <c s="14"/>
+      <c s="14"/>
+      <c s="2" t="s">
+        <v>88</v>
       </c>
       <c s="2" t="s">
         <v>45</v>
@@ -3089,13 +3201,13 @@
       <c s="1"/>
     </row>
     <row>
-      <c s="20"/>
-      <c s="20"/>
-      <c s="2" t="s">
-        <v>21</v>
-      </c>
-      <c s="2" t="s">
-        <v>78</v>
+      <c s="14"/>
+      <c s="14"/>
+      <c s="2" t="s">
+        <v>20</v>
+      </c>
+      <c s="2" t="s">
+        <v>79</v>
       </c>
       <c s="2"/>
       <c s="2" t="s">
@@ -3104,37 +3216,37 @@
       <c s="1"/>
     </row>
     <row>
-      <c s="20"/>
-      <c s="20"/>
+      <c s="14"/>
+      <c s="14"/>
       <c s="2" t="s">
         <v>43</v>
       </c>
       <c s="2" t="s">
-        <v>91</v>
-      </c>
-      <c s="2"/>
-      <c s="2"/>
-      <c s="1"/>
-    </row>
-    <row>
-      <c s="20"/>
-      <c s="20"/>
+        <v>93</v>
+      </c>
+      <c s="2"/>
+      <c s="2"/>
+      <c s="1"/>
+    </row>
+    <row>
+      <c s="14"/>
+      <c s="14"/>
       <c s="2" t="s">
         <v>69</v>
       </c>
       <c s="12" t="s">
-        <v>76</v>
-      </c>
-      <c s="2"/>
-      <c s="2"/>
-      <c s="1"/>
-    </row>
-    <row>
-      <c s="20" t="s">
+        <v>77</v>
+      </c>
+      <c s="2"/>
+      <c s="2"/>
+      <c s="1"/>
+    </row>
+    <row>
+      <c s="14" t="s">
         <v>55</v>
       </c>
-      <c s="20" t="s">
-        <v>17</v>
+      <c s="14" t="s">
+        <v>16</v>
       </c>
       <c s="2" t="s">
         <v>67</v>
@@ -3149,10 +3261,10 @@
       <c s="1"/>
     </row>
     <row>
-      <c s="20"/>
-      <c s="20"/>
-      <c s="2" t="s">
-        <v>86</v>
+      <c s="14"/>
+      <c s="14"/>
+      <c s="2" t="s">
+        <v>88</v>
       </c>
       <c s="2" t="s">
         <v>45</v>
@@ -3162,13 +3274,13 @@
       <c s="1"/>
     </row>
     <row>
-      <c s="20"/>
-      <c s="20"/>
-      <c s="2" t="s">
-        <v>21</v>
-      </c>
-      <c s="2" t="s">
-        <v>78</v>
+      <c s="14"/>
+      <c s="14"/>
+      <c s="2" t="s">
+        <v>20</v>
+      </c>
+      <c s="2" t="s">
+        <v>79</v>
       </c>
       <c s="2"/>
       <c s="2" t="s">
@@ -3177,37 +3289,37 @@
       <c s="1"/>
     </row>
     <row>
-      <c s="20"/>
-      <c s="20"/>
+      <c s="14"/>
+      <c s="14"/>
       <c s="2" t="s">
         <v>43</v>
       </c>
       <c s="2" t="s">
-        <v>91</v>
-      </c>
-      <c s="2"/>
-      <c s="2"/>
-      <c s="1"/>
-    </row>
-    <row>
-      <c s="20"/>
-      <c s="20"/>
+        <v>93</v>
+      </c>
+      <c s="2"/>
+      <c s="2"/>
+      <c s="1"/>
+    </row>
+    <row>
+      <c s="14"/>
+      <c s="14"/>
       <c s="2" t="s">
         <v>69</v>
       </c>
       <c s="12" t="s">
-        <v>76</v>
-      </c>
-      <c s="2"/>
-      <c s="2"/>
-      <c s="1"/>
-    </row>
-    <row>
-      <c s="20" t="s">
+        <v>77</v>
+      </c>
+      <c s="2"/>
+      <c s="2"/>
+      <c s="1"/>
+    </row>
+    <row>
+      <c s="14" t="s">
         <v>70</v>
       </c>
-      <c s="20" t="s">
-        <v>28</v>
+      <c s="14" t="s">
+        <v>27</v>
       </c>
       <c s="1" t="s">
         <v>67</v>
@@ -3222,10 +3334,10 @@
       <c s="1"/>
     </row>
     <row>
-      <c s="20"/>
-      <c s="20"/>
-      <c s="1" t="s">
-        <v>86</v>
+      <c s="14"/>
+      <c s="14"/>
+      <c s="1" t="s">
+        <v>88</v>
       </c>
       <c s="1" t="s">
         <v>45</v>
@@ -3235,13 +3347,13 @@
       <c s="1"/>
     </row>
     <row>
-      <c s="20"/>
-      <c s="20"/>
-      <c s="1" t="s">
-        <v>21</v>
-      </c>
-      <c s="1" t="s">
-        <v>78</v>
+      <c s="14"/>
+      <c s="14"/>
+      <c s="1" t="s">
+        <v>20</v>
+      </c>
+      <c s="1" t="s">
+        <v>79</v>
       </c>
       <c s="1"/>
       <c s="1" t="s">
@@ -3250,26 +3362,26 @@
       <c s="1"/>
     </row>
     <row>
-      <c s="20"/>
-      <c s="20"/>
+      <c s="14"/>
+      <c s="14"/>
       <c s="1" t="s">
         <v>43</v>
       </c>
       <c s="1" t="s">
+        <v>73</v>
+      </c>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+    </row>
+    <row>
+      <c s="14"/>
+      <c s="14"/>
+      <c s="1" t="s">
+        <v>1</v>
+      </c>
+      <c s="1" t="s">
         <v>72</v>
-      </c>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-    </row>
-    <row>
-      <c s="20"/>
-      <c s="20"/>
-      <c s="1" t="s">
-        <v>1</v>
-      </c>
-      <c s="1" t="s">
-        <v>71</v>
       </c>
       <c s="1"/>
       <c s="1"/>
@@ -3280,7 +3392,7 @@
         <v>40</v>
       </c>
       <c s="16" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c s="2" t="s">
         <v>67</v>
@@ -3298,7 +3410,7 @@
       <c s="16"/>
       <c s="16"/>
       <c s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c s="2" t="s">
         <v>45</v>
@@ -3311,10 +3423,10 @@
       <c s="16"/>
       <c s="16"/>
       <c s="2" t="s">
-        <v>21</v>
-      </c>
-      <c s="2" t="s">
-        <v>78</v>
+        <v>20</v>
+      </c>
+      <c s="2" t="s">
+        <v>79</v>
       </c>
       <c s="1"/>
       <c s="1" t="s">
@@ -3329,7 +3441,7 @@
         <v>43</v>
       </c>
       <c s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c s="1"/>
       <c s="1"/>
@@ -3342,7 +3454,7 @@
         <v>69</v>
       </c>
       <c s="12" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c s="1"/>
       <c s="1"/>
@@ -3350,7 +3462,7 @@
     </row>
     <row>
       <c s="16" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c s="16" t="s">
         <v>46</v>
@@ -3362,7 +3474,7 @@
         <v>30</v>
       </c>
       <c s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c s="1"/>
       <c s="1"/>
@@ -3371,7 +3483,7 @@
       <c s="16"/>
       <c s="16"/>
       <c s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c s="1" t="s">
         <v>45</v>
@@ -3384,10 +3496,10 @@
       <c s="16"/>
       <c s="16"/>
       <c s="1" t="s">
-        <v>21</v>
-      </c>
-      <c s="1" t="s">
-        <v>78</v>
+        <v>20</v>
+      </c>
+      <c s="1" t="s">
+        <v>79</v>
       </c>
       <c s="1"/>
       <c s="1" t="s">
@@ -3402,7 +3514,7 @@
         <v>43</v>
       </c>
       <c s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c s="1"/>
       <c s="1"/>
@@ -3415,7 +3527,7 @@
         <v>1</v>
       </c>
       <c s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c s="1"/>
       <c s="1"/>
@@ -3423,10 +3535,10 @@
     </row>
     <row>
       <c s="16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c s="1" t="s">
         <v>67</v>
@@ -3435,7 +3547,7 @@
         <v>30</v>
       </c>
       <c s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c s="1"/>
       <c s="1"/>
@@ -3444,7 +3556,7 @@
       <c s="16"/>
       <c s="16"/>
       <c s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c s="1" t="s">
         <v>45</v>
@@ -3457,10 +3569,10 @@
       <c s="16"/>
       <c s="16"/>
       <c s="1" t="s">
-        <v>21</v>
-      </c>
-      <c s="1" t="s">
-        <v>78</v>
+        <v>20</v>
+      </c>
+      <c s="1" t="s">
+        <v>79</v>
       </c>
       <c s="1"/>
       <c s="1" t="s">
@@ -3475,7 +3587,7 @@
         <v>43</v>
       </c>
       <c s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c s="1"/>
       <c s="1"/>
@@ -3504,7 +3616,7 @@
       <c s="16"/>
       <c s="16"/>
       <c s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c s="1" t="s">
         <v>45</v>
@@ -3517,10 +3629,10 @@
       <c s="16"/>
       <c s="16"/>
       <c s="1" t="s">
-        <v>21</v>
-      </c>
-      <c s="1" t="s">
-        <v>71</v>
+        <v>20</v>
+      </c>
+      <c s="1" t="s">
+        <v>72</v>
       </c>
       <c s="1"/>
       <c s="1"/>
@@ -3575,10 +3687,10 @@
         <v>0</v>
       </c>
       <c s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c s="4" t="s">
         <v>36</v>
@@ -3588,57 +3700,57 @@
       </c>
     </row>
     <row>
-      <c s="10" t="s">
+      <c s="8" t="s">
+        <v>80</v>
+      </c>
+      <c s="3" t="s">
+        <v>58</v>
+      </c>
+      <c s="1" t="s">
+        <v>67</v>
+      </c>
+      <c s="1" t="s">
+        <v>30</v>
+      </c>
+      <c s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G2" s="1"/>
+    </row>
+    <row>
+      <c s="8"/>
+      <c s="3"/>
+      <c s="1" t="s">
+        <v>88</v>
+      </c>
+      <c s="1" t="s">
+        <v>38</v>
+      </c>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+    </row>
+    <row>
+      <c s="8"/>
+      <c s="3"/>
+      <c s="1" t="s">
+        <v>20</v>
+      </c>
+      <c s="1" t="s">
+        <v>14</v>
+      </c>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+    </row>
+    <row>
+      <c s="8"/>
+      <c s="3"/>
+      <c s="1" t="s">
+        <v>43</v>
+      </c>
+      <c s="1" t="s">
         <v>79</v>
-      </c>
-      <c s="3" t="s">
-        <v>58</v>
-      </c>
-      <c s="1" t="s">
-        <v>67</v>
-      </c>
-      <c s="1" t="s">
-        <v>30</v>
-      </c>
-      <c s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="G2" s="1"/>
-    </row>
-    <row>
-      <c s="10"/>
-      <c s="3"/>
-      <c s="1" t="s">
-        <v>86</v>
-      </c>
-      <c s="1" t="s">
-        <v>38</v>
-      </c>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-    </row>
-    <row>
-      <c s="10"/>
-      <c s="3"/>
-      <c s="1" t="s">
-        <v>21</v>
-      </c>
-      <c s="1" t="s">
-        <v>15</v>
-      </c>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-    </row>
-    <row>
-      <c s="10"/>
-      <c s="3"/>
-      <c s="1" t="s">
-        <v>43</v>
-      </c>
-      <c s="1" t="s">
-        <v>78</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>68</v>
@@ -3646,20 +3758,20 @@
       <c s="1"/>
     </row>
     <row>
-      <c s="10"/>
+      <c s="8"/>
       <c s="3"/>
       <c s="1" t="s">
         <v>69</v>
       </c>
       <c t="s">
-        <v>24</v>
-      </c>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-    </row>
-    <row>
-      <c s="10" t="s">
+        <v>23</v>
+      </c>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+    </row>
+    <row>
+      <c s="8" t="s">
         <v>31</v>
       </c>
       <c s="9" t="s">
@@ -3678,10 +3790,10 @@
       <c s="2"/>
     </row>
     <row>
-      <c s="10"/>
+      <c s="8"/>
       <c s="9"/>
       <c s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c t="s">
         <v>4</v>
@@ -3693,24 +3805,24 @@
       <c s="2"/>
     </row>
     <row>
-      <c s="10"/>
+      <c s="8"/>
       <c s="9"/>
       <c s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c t="s">
-        <v>24</v>
-      </c>
-      <c s="2"/>
-      <c s="2"/>
-      <c s="2"/>
-    </row>
-    <row>
-      <c s="10" t="s">
+        <v>23</v>
+      </c>
+      <c s="2"/>
+      <c s="2"/>
+      <c s="2"/>
+    </row>
+    <row>
+      <c s="8" t="s">
         <v>53</v>
       </c>
       <c s="9" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c s="2" t="s">
         <v>67</v>
@@ -3725,10 +3837,10 @@
       <c s="2"/>
     </row>
     <row>
-      <c s="10"/>
+      <c s="8"/>
       <c s="9"/>
       <c s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c t="s">
         <v>4</v>
@@ -3740,24 +3852,24 @@
       <c s="2"/>
     </row>
     <row>
-      <c s="10"/>
+      <c s="8"/>
       <c s="9"/>
       <c s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c t="s">
-        <v>24</v>
-      </c>
-      <c s="2"/>
-      <c s="2"/>
-      <c s="2"/>
-    </row>
-    <row>
-      <c s="15" t="s">
-        <v>80</v>
-      </c>
-      <c s="22" t="s">
-        <v>16</v>
+        <v>23</v>
+      </c>
+      <c s="2"/>
+      <c s="2"/>
+      <c s="2"/>
+    </row>
+    <row>
+      <c s="13" t="s">
+        <v>81</v>
+      </c>
+      <c s="20" t="s">
+        <v>15</v>
       </c>
       <c s="2" t="s">
         <v>67</v>
@@ -3766,16 +3878,16 @@
         <v>30</v>
       </c>
       <c s="2" t="s">
-        <v>80</v>
-      </c>
-      <c s="2"/>
-      <c s="2"/>
-    </row>
-    <row>
-      <c s="13"/>
-      <c s="17"/>
-      <c s="2" t="s">
-        <v>86</v>
+        <v>81</v>
+      </c>
+      <c s="2"/>
+      <c s="2"/>
+    </row>
+    <row>
+      <c s="22"/>
+      <c s="21"/>
+      <c s="2" t="s">
+        <v>88</v>
       </c>
       <c t="s">
         <v>4</v>
@@ -3787,21 +3899,21 @@
       <c s="2"/>
     </row>
     <row>
-      <c s="13"/>
-      <c s="17"/>
-      <c s="2" t="s">
-        <v>21</v>
-      </c>
-      <c s="1" t="s">
-        <v>24</v>
-      </c>
-      <c s="2"/>
-      <c s="2"/>
-      <c s="2"/>
-    </row>
-    <row>
-      <c s="13"/>
-      <c s="17"/>
+      <c s="22"/>
+      <c s="21"/>
+      <c s="2" t="s">
+        <v>20</v>
+      </c>
+      <c s="1" t="s">
+        <v>23</v>
+      </c>
+      <c s="2"/>
+      <c s="2"/>
+      <c s="2"/>
+    </row>
+    <row>
+      <c s="22"/>
+      <c s="21"/>
       <c s="2" t="s">
         <v>43</v>
       </c>
@@ -3815,8 +3927,8 @@
       <c s="2"/>
     </row>
     <row>
-      <c s="13"/>
-      <c s="17"/>
+      <c s="22"/>
+      <c s="21"/>
       <c s="2" t="s">
         <v>69</v>
       </c>
@@ -3824,15 +3936,15 @@
         <v>59</v>
       </c>
       <c s="1"/>
-      <c s="11"/>
-      <c s="2"/>
-    </row>
-    <row>
-      <c s="10" t="s">
+      <c s="10"/>
+      <c s="2"/>
+    </row>
+    <row>
+      <c s="8" t="s">
         <v>8</v>
       </c>
       <c s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c s="2" t="s">
         <v>67</v>
@@ -3847,10 +3959,10 @@
       <c s="2"/>
     </row>
     <row>
-      <c s="10"/>
+      <c s="8"/>
       <c s="9"/>
       <c s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c t="s">
         <v>4</v>
@@ -3862,20 +3974,20 @@
       <c s="2"/>
     </row>
     <row>
-      <c s="10"/>
+      <c s="8"/>
       <c s="9"/>
       <c s="2" t="s">
-        <v>21</v>
-      </c>
-      <c s="1" t="s">
-        <v>24</v>
-      </c>
-      <c s="2"/>
-      <c s="2"/>
-      <c s="2"/>
-    </row>
-    <row>
-      <c s="10"/>
+        <v>20</v>
+      </c>
+      <c s="1" t="s">
+        <v>23</v>
+      </c>
+      <c s="2"/>
+      <c s="2"/>
+      <c s="2"/>
+    </row>
+    <row>
+      <c s="8"/>
       <c s="9"/>
       <c s="2" t="s">
         <v>43</v>
@@ -3890,41 +4002,41 @@
       <c s="2"/>
     </row>
     <row>
+      <c s="8"/>
+      <c s="9"/>
+      <c s="2" t="s">
+        <v>69</v>
+      </c>
+      <c s="1" t="s">
+        <v>59</v>
+      </c>
+      <c s="1"/>
       <c s="10"/>
+      <c s="2"/>
+    </row>
+    <row>
+      <c s="8"/>
       <c s="9"/>
       <c s="2" t="s">
-        <v>69</v>
-      </c>
-      <c s="1" t="s">
-        <v>59</v>
-      </c>
-      <c s="1"/>
-      <c s="11"/>
-      <c s="2"/>
-    </row>
-    <row>
-      <c s="10"/>
+        <v>91</v>
+      </c>
+      <c s="1" t="s">
+        <v>62</v>
+      </c>
+      <c s="2"/>
+      <c s="2" t="s">
+        <v>26</v>
+      </c>
+      <c s="2"/>
+    </row>
+    <row>
+      <c s="8"/>
       <c s="9"/>
       <c s="2" t="s">
-        <v>89</v>
-      </c>
-      <c s="1" t="s">
-        <v>62</v>
-      </c>
-      <c s="2"/>
-      <c s="2" t="s">
-        <v>27</v>
-      </c>
-      <c s="2"/>
-    </row>
-    <row>
-      <c s="10"/>
-      <c s="9"/>
-      <c s="2" t="s">
-        <v>26</v>
-      </c>
-      <c s="1" t="s">
-        <v>74</v>
+        <v>25</v>
+      </c>
+      <c s="1" t="s">
+        <v>75</v>
       </c>
       <c s="2"/>
       <c s="2"/>
@@ -3953,7 +4065,7 @@
       <c s="7"/>
       <c s="7"/>
       <c s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c s="1" t="s">
         <v>4</v>
@@ -3968,10 +4080,10 @@
       <c s="7"/>
       <c s="7"/>
       <c s="2" t="s">
-        <v>21</v>
-      </c>
-      <c s="1" t="s">
-        <v>24</v>
+        <v>20</v>
+      </c>
+      <c s="1" t="s">
+        <v>23</v>
       </c>
       <c s="2"/>
       <c s="2"/>
@@ -4009,22 +4121,22 @@
       <c s="7"/>
       <c s="7"/>
       <c s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c s="1" t="s">
         <v>62</v>
       </c>
       <c s="2"/>
       <c s="2" t="s">
-        <v>27</v>
-      </c>
-      <c s="1"/>
-    </row>
-    <row>
-      <c s="7"/>
-      <c s="7"/>
-      <c s="2" t="s">
         <v>26</v>
+      </c>
+      <c s="1"/>
+    </row>
+    <row>
+      <c s="7"/>
+      <c s="7"/>
+      <c s="2" t="s">
+        <v>25</v>
       </c>
       <c s="1" t="s">
         <v>50</v>
@@ -4056,7 +4168,7 @@
       <c s="7"/>
       <c s="7"/>
       <c s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c s="1" t="s">
         <v>4</v>
@@ -4071,10 +4183,10 @@
       <c s="7"/>
       <c s="7"/>
       <c s="2" t="s">
-        <v>21</v>
-      </c>
-      <c s="1" t="s">
-        <v>24</v>
+        <v>20</v>
+      </c>
+      <c s="1" t="s">
+        <v>23</v>
       </c>
       <c s="2"/>
       <c s="2"/>
@@ -4112,25 +4224,25 @@
       <c s="7"/>
       <c s="7"/>
       <c s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c s="1" t="s">
         <v>62</v>
       </c>
       <c s="2"/>
       <c s="2" t="s">
-        <v>27</v>
-      </c>
-      <c s="1"/>
-    </row>
-    <row>
-      <c s="7"/>
-      <c s="7"/>
-      <c s="2" t="s">
         <v>26</v>
       </c>
-      <c s="1" t="s">
-        <v>18</v>
+      <c s="1"/>
+    </row>
+    <row>
+      <c s="7"/>
+      <c s="7"/>
+      <c s="2" t="s">
+        <v>25</v>
+      </c>
+      <c s="1" t="s">
+        <v>17</v>
       </c>
       <c s="1"/>
       <c s="1"/>
@@ -4159,7 +4271,7 @@
       <c s="7"/>
       <c s="7"/>
       <c s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c s="1" t="s">
         <v>4</v>
@@ -4174,7 +4286,7 @@
       <c s="7"/>
       <c s="7"/>
       <c s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c s="1" t="s">
         <v>47</v>
@@ -4206,7 +4318,7 @@
       <c s="7"/>
       <c s="7"/>
       <c s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c s="1" t="s">
         <v>4</v>
@@ -4221,7 +4333,7 @@
       <c s="7"/>
       <c s="7"/>
       <c s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c s="1" t="s">
         <v>47</v>
@@ -4234,7 +4346,7 @@
       <c s="3" t="s">
         <v>10</v>
       </c>
-      <c s="19" t="s">
+      <c s="15" t="s">
         <v>64</v>
       </c>
       <c s="3" t="s">
@@ -4251,9 +4363,9 @@
     </row>
     <row>
       <c s="3"/>
-      <c s="19"/>
-      <c s="3" t="s">
-        <v>86</v>
+      <c s="15"/>
+      <c s="3" t="s">
+        <v>88</v>
       </c>
       <c s="1" t="s">
         <v>4</v>
@@ -4266,13 +4378,13 @@
     </row>
     <row>
       <c s="3"/>
-      <c s="19"/>
-      <c s="3" t="s">
-        <v>21</v>
-      </c>
-      <c s="1" t="s">
+      <c s="15"/>
+      <c s="3" t="s">
         <v>20</v>
       </c>
+      <c s="1" t="s">
+        <v>19</v>
+      </c>
       <c s="1"/>
       <c s="3" t="s">
         <v>65</v>
@@ -4281,7 +4393,7 @@
     </row>
     <row>
       <c s="3"/>
-      <c s="19"/>
+      <c s="15"/>
       <c s="3" t="s">
         <v>43</v>
       </c>
@@ -4296,38 +4408,38 @@
     </row>
     <row>
       <c s="3"/>
-      <c s="19"/>
+      <c s="15"/>
       <c s="3" t="s">
         <v>69</v>
       </c>
       <c s="1" t="s">
-        <v>24</v>
-      </c>
-      <c s="3"/>
-      <c s="1"/>
-      <c s="3"/>
-    </row>
-    <row>
-      <c s="3"/>
-      <c s="19"/>
-      <c s="3" t="s">
-        <v>89</v>
+        <v>23</v>
+      </c>
+      <c s="3"/>
+      <c s="1"/>
+      <c s="3"/>
+    </row>
+    <row>
+      <c s="3"/>
+      <c s="15"/>
+      <c s="3" t="s">
+        <v>91</v>
       </c>
       <c s="1" t="s">
         <v>62</v>
       </c>
       <c s="3"/>
       <c s="3" t="s">
-        <v>27</v>
-      </c>
-      <c s="3"/>
-    </row>
-    <row>
-      <c s="3"/>
-      <c s="19"/>
-      <c s="3" t="s">
         <v>26</v>
       </c>
+      <c s="3"/>
+    </row>
+    <row>
+      <c s="3"/>
+      <c s="15"/>
+      <c s="3" t="s">
+        <v>25</v>
+      </c>
       <c s="1" t="s">
         <v>59</v>
       </c>
@@ -4337,7 +4449,7 @@
     </row>
     <row>
       <c s="3"/>
-      <c s="19"/>
+      <c s="15"/>
       <c s="3" t="s">
         <v>49</v>
       </c>
@@ -4352,20 +4464,20 @@
     </row>
     <row>
       <c s="3"/>
-      <c s="19"/>
-      <c s="3" t="s">
-        <v>73</v>
-      </c>
-      <c s="3" t="s">
-        <v>77</v>
-      </c>
-      <c s="3"/>
-      <c s="3"/>
-      <c s="3"/>
-    </row>
-    <row>
-      <c s="3"/>
-      <c s="19"/>
+      <c s="15"/>
+      <c s="3" t="s">
+        <v>74</v>
+      </c>
+      <c s="3" t="s">
+        <v>78</v>
+      </c>
+      <c s="3"/>
+      <c s="3"/>
+      <c s="3"/>
+    </row>
+    <row>
+      <c s="3"/>
+      <c s="15"/>
       <c s="3" t="s">
         <v>7</v>
       </c>
@@ -4380,86 +4492,86 @@
     </row>
     <row>
       <c s="3"/>
-      <c s="19"/>
+      <c s="15"/>
       <c s="3" t="s">
         <v>32</v>
       </c>
       <c s="3" t="s">
+        <v>19</v>
+      </c>
+      <c s="3"/>
+      <c s="3" t="s">
+        <v>42</v>
+      </c>
+      <c s="3"/>
+    </row>
+    <row>
+      <c s="3"/>
+      <c s="15"/>
+      <c s="3" t="s">
+        <v>60</v>
+      </c>
+      <c s="1" t="s">
+        <v>62</v>
+      </c>
+      <c s="3"/>
+      <c s="3" t="s">
+        <v>26</v>
+      </c>
+      <c s="3"/>
+    </row>
+    <row>
+      <c s="3"/>
+      <c s="15"/>
+      <c s="3" t="s">
+        <v>87</v>
+      </c>
+      <c s="3" t="s">
+        <v>6</v>
+      </c>
+      <c s="3"/>
+      <c s="3"/>
+      <c s="3"/>
+    </row>
+    <row>
+      <c s="3" t="s">
+        <v>35</v>
+      </c>
+      <c s="15" t="s">
+        <v>48</v>
+      </c>
+      <c s="3" t="s">
+        <v>67</v>
+      </c>
+      <c s="3" t="s">
+        <v>30</v>
+      </c>
+      <c s="3" t="s">
+        <v>35</v>
+      </c>
+      <c s="3"/>
+      <c s="3"/>
+    </row>
+    <row>
+      <c s="3"/>
+      <c s="15"/>
+      <c s="3" t="s">
+        <v>88</v>
+      </c>
+      <c s="1" t="s">
+        <v>4</v>
+      </c>
+      <c s="17"/>
+      <c s="3" t="s">
+        <v>68</v>
+      </c>
+      <c s="3"/>
+    </row>
+    <row>
+      <c s="3"/>
+      <c s="15"/>
+      <c s="3" t="s">
         <v>20</v>
-      </c>
-      <c s="3"/>
-      <c s="3" t="s">
-        <v>42</v>
-      </c>
-      <c s="3"/>
-    </row>
-    <row>
-      <c s="3"/>
-      <c s="19"/>
-      <c s="3" t="s">
-        <v>60</v>
-      </c>
-      <c s="1" t="s">
-        <v>62</v>
-      </c>
-      <c s="3"/>
-      <c s="3" t="s">
-        <v>27</v>
-      </c>
-      <c s="3"/>
-    </row>
-    <row>
-      <c s="3"/>
-      <c s="19"/>
-      <c s="3" t="s">
-        <v>85</v>
-      </c>
-      <c s="3" t="s">
-        <v>6</v>
-      </c>
-      <c s="3"/>
-      <c s="3"/>
-      <c s="3"/>
-    </row>
-    <row>
-      <c s="3" t="s">
-        <v>35</v>
-      </c>
-      <c s="19" t="s">
-        <v>48</v>
-      </c>
-      <c s="3" t="s">
-        <v>67</v>
-      </c>
-      <c s="3" t="s">
-        <v>30</v>
-      </c>
-      <c s="3" t="s">
-        <v>35</v>
-      </c>
-      <c s="3"/>
-      <c s="3"/>
-    </row>
-    <row>
-      <c s="3"/>
-      <c s="19"/>
-      <c s="3" t="s">
-        <v>86</v>
-      </c>
-      <c s="1" t="s">
-        <v>4</v>
-      </c>
-      <c s="21"/>
-      <c s="3" t="s">
-        <v>68</v>
-      </c>
-      <c s="3"/>
-    </row>
-    <row>
-      <c s="3"/>
-      <c s="19"/>
-      <c s="3" t="s">
-        <v>21</v>
       </c>
       <c s="3" t="s">
         <v>66</v>
@@ -4473,7 +4585,7 @@
         <v>57</v>
       </c>
       <c s="7" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c s="2" t="s">
         <v>67</v>
@@ -4491,7 +4603,7 @@
       <c s="7"/>
       <c s="7"/>
       <c s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c s="1" t="s">
         <v>4</v>
@@ -4506,10 +4618,10 @@
       <c s="7"/>
       <c s="7"/>
       <c s="2" t="s">
-        <v>21</v>
-      </c>
-      <c s="1" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c s="1" t="s">
+        <v>18</v>
       </c>
       <c s="1"/>
       <c s="1"/>

</xml_diff>